<commit_message>
add test case in test suite folder
</commit_message>
<xml_diff>
--- a/autolist.xlsx
+++ b/autolist.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D919FD-D058-4B1F-91E0-C48BF724ABEC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11745"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="17616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="160">
   <si>
     <t>01.Application</t>
   </si>
@@ -507,7 +508,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,25 +902,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="107.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="107.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>155</v>
       </c>
@@ -941,14 +942,16 @@
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D2" s="5" t="s">
         <v>158</v>
       </c>
@@ -959,12 +962,14 @@
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>158</v>
       </c>
@@ -975,7 +980,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -991,12 +996,14 @@
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>158</v>
       </c>
@@ -1007,12 +1014,14 @@
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>158</v>
       </c>
@@ -1023,12 +1032,14 @@
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D7" s="5" t="s">
         <v>158</v>
       </c>
@@ -1039,12 +1050,14 @@
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>158</v>
       </c>
@@ -1055,12 +1068,14 @@
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>158</v>
       </c>
@@ -1071,7 +1086,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -1087,7 +1102,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -1105,7 +1120,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="6" t="s">
         <v>14</v>
@@ -1123,7 +1138,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>15</v>
@@ -1141,7 +1156,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>89</v>
       </c>
@@ -1159,7 +1174,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>90</v>
@@ -1175,7 +1190,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="6" t="s">
         <v>91</v>
@@ -1191,7 +1206,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>92</v>
@@ -1207,7 +1222,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="6" t="s">
         <v>93</v>
@@ -1223,7 +1238,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
         <v>94</v>
@@ -1239,7 +1254,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="6" t="s">
         <v>95</v>
@@ -1255,7 +1270,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>96</v>
       </c>
@@ -1275,7 +1290,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
         <v>98</v>
@@ -1293,7 +1308,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
         <v>99</v>
@@ -1311,7 +1326,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
         <v>100</v>
@@ -1329,7 +1344,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>101</v>
@@ -1347,7 +1362,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6" t="s">
         <v>102</v>
@@ -1365,7 +1380,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6" t="s">
         <v>103</v>
@@ -1383,7 +1398,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>104</v>
@@ -1401,7 +1416,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
         <v>105</v>
@@ -1419,7 +1434,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
         <v>106</v>
@@ -1437,7 +1452,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>107</v>
       </c>
@@ -1455,7 +1470,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
         <v>109</v>
@@ -1471,7 +1486,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
         <v>110</v>
@@ -1487,7 +1502,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
         <v>111</v>
@@ -1503,7 +1518,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
         <v>112</v>
@@ -1519,7 +1534,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>113</v>
@@ -1535,7 +1550,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
         <v>114</v>
@@ -1551,7 +1566,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="6" t="s">
         <v>115</v>
@@ -1567,7 +1582,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>116</v>
       </c>
@@ -1585,7 +1600,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="4" t="s">
         <v>118</v>
@@ -1601,7 +1616,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="6" t="s">
         <v>119</v>
@@ -1617,7 +1632,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>120</v>
@@ -1633,7 +1648,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
         <v>121</v>
@@ -1649,7 +1664,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="6" t="s">
         <v>122</v>
@@ -1665,7 +1680,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="6" t="s">
         <v>123</v>
@@ -1681,7 +1696,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="6" t="s">
         <v>124</v>
@@ -1697,7 +1712,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="4" t="s">
         <v>125</v>
@@ -1713,7 +1728,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
         <v>126</v>
@@ -1729,7 +1744,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="4" t="s">
         <v>127</v>
@@ -1745,7 +1760,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
         <v>128</v>
@@ -1761,7 +1776,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>129</v>
@@ -1777,7 +1792,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
         <v>130</v>
@@ -1793,7 +1808,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
         <v>131</v>
@@ -1809,7 +1824,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="6" t="s">
         <v>132</v>
@@ -1825,7 +1840,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="4" t="s">
         <v>133</v>
@@ -1841,7 +1856,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="4" t="s">
         <v>134</v>
@@ -1857,7 +1872,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
         <v>135</v>
@@ -1873,7 +1888,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="4" t="s">
         <v>153</v>
@@ -1889,7 +1904,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>136</v>
       </c>
@@ -1907,7 +1922,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
         <v>138</v>
@@ -1923,7 +1938,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="6" t="s">
         <v>139</v>
@@ -1939,7 +1954,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
         <v>140</v>
@@ -1955,7 +1970,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>87</v>
       </c>
@@ -1973,7 +1988,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="6" t="s">
         <v>142</v>
@@ -1989,7 +2004,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="4" t="s">
         <v>143</v>
@@ -2005,7 +2020,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="6" t="s">
         <v>144</v>
@@ -2021,7 +2036,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
         <v>145</v>
@@ -2037,7 +2052,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="4" t="s">
         <v>146</v>
@@ -2053,7 +2068,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
         <v>147</v>
@@ -2069,7 +2084,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>16</v>
       </c>
@@ -2087,7 +2102,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="4" t="s">
         <v>149</v>
@@ -2103,7 +2118,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
         <v>150</v>
@@ -2119,7 +2134,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>17</v>
       </c>
@@ -2139,7 +2154,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
         <v>19</v>
@@ -2157,7 +2172,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
         <v>20</v>
@@ -2175,7 +2190,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="4" t="s">
         <v>21</v>
@@ -2193,7 +2208,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>35</v>
       </c>
@@ -2213,7 +2228,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
         <v>23</v>
@@ -2231,7 +2246,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="4" t="s">
         <v>24</v>
@@ -2249,7 +2264,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="4" t="s">
         <v>25</v>
@@ -2267,7 +2282,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
         <v>26</v>
@@ -2285,7 +2300,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="4" t="s">
         <v>27</v>
@@ -2303,7 +2318,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="4" t="s">
         <v>28</v>
@@ -2321,7 +2336,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="4" t="s">
         <v>29</v>
@@ -2339,7 +2354,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>36</v>
       </c>
@@ -2359,7 +2374,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="4" t="s">
         <v>34</v>
@@ -2377,7 +2392,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>37</v>
       </c>
@@ -2397,7 +2412,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="4" t="s">
         <v>39</v>
@@ -2415,7 +2430,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>40</v>
       </c>
@@ -2435,7 +2450,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="4" t="s">
         <v>42</v>
@@ -2453,7 +2468,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="4" t="s">
         <v>43</v>
@@ -2471,7 +2486,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="4" t="s">
         <v>44</v>
@@ -2489,7 +2504,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>45</v>
       </c>
@@ -2509,7 +2524,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="4" t="s">
         <v>46</v>
@@ -2527,7 +2542,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="4" t="s">
         <v>47</v>
@@ -2545,7 +2560,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="6" t="s">
         <v>48</v>
@@ -2563,7 +2578,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="4" t="s">
         <v>49</v>
@@ -2581,7 +2596,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="4" t="s">
         <v>50</v>
@@ -2599,7 +2614,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="6" t="s">
         <v>51</v>
@@ -2617,7 +2632,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="6" t="s">
         <v>52</v>
@@ -2635,7 +2650,7 @@
       <c r="G100" s="2"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="6" t="s">
         <v>53</v>
@@ -2653,7 +2668,7 @@
       <c r="G101" s="2"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="6" t="s">
         <v>152</v>
@@ -2671,7 +2686,7 @@
       <c r="G102" s="2"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>55</v>
       </c>
@@ -2691,7 +2706,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>56</v>
       </c>
@@ -2711,7 +2726,7 @@
       <c r="G104" s="2"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="4" t="s">
         <v>62</v>
@@ -2729,7 +2744,7 @@
       <c r="G105" s="2"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>63</v>
       </c>
@@ -2749,7 +2764,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="4" t="s">
         <v>58</v>
@@ -2767,7 +2782,7 @@
       <c r="G107" s="2"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="6" t="s">
         <v>59</v>
@@ -2785,7 +2800,7 @@
       <c r="G108" s="2"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>60</v>
       </c>
@@ -2805,7 +2820,7 @@
       <c r="G109" s="2"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="6" t="s">
         <v>65</v>
@@ -2823,7 +2838,7 @@
       <c r="G110" s="2"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="4" t="s">
         <v>66</v>
@@ -2841,7 +2856,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="4" t="s">
         <v>67</v>
@@ -2859,7 +2874,7 @@
       <c r="G112" s="2"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="6" t="s">
         <v>68</v>
@@ -2877,7 +2892,7 @@
       <c r="G113" s="2"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="6" t="s">
         <v>69</v>
@@ -2895,7 +2910,7 @@
       <c r="G114" s="2"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="6" t="s">
         <v>70</v>
@@ -2913,7 +2928,7 @@
       <c r="G115" s="2"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="6" t="s">
         <v>71</v>
@@ -2931,7 +2946,7 @@
       <c r="G116" s="2"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="4" t="s">
         <v>72</v>
@@ -2949,7 +2964,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="6" t="s">
         <v>73</v>
@@ -2967,7 +2982,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="4" t="s">
         <v>74</v>
@@ -2985,7 +3000,7 @@
       <c r="G119" s="2"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="4" t="s">
         <v>75</v>
@@ -3003,7 +3018,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="6" t="s">
         <v>76</v>
@@ -3021,7 +3036,7 @@
       <c r="G121" s="2"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="6" t="s">
         <v>77</v>
@@ -3039,7 +3054,7 @@
       <c r="G122" s="2"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="6" t="s">
         <v>78</v>
@@ -3057,7 +3072,7 @@
       <c r="G123" s="2"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="6" t="s">
         <v>79</v>
@@ -3075,7 +3090,7 @@
       <c r="G124" s="2"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="6" t="s">
         <v>80</v>
@@ -3093,7 +3108,7 @@
       <c r="G125" s="2"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="4" t="s">
         <v>81</v>
@@ -3111,7 +3126,7 @@
       <c r="G126" s="2"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="4" t="s">
         <v>82</v>
@@ -3129,7 +3144,7 @@
       <c r="G127" s="2"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="4" t="s">
         <v>83</v>
@@ -3147,7 +3162,7 @@
       <c r="G128" s="2"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="4" t="s">
         <v>84</v>
@@ -3165,7 +3180,7 @@
       <c r="G129" s="2"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="4" t="s">
         <v>85</v>
@@ -3183,7 +3198,7 @@
       <c r="G130" s="2"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="4" t="s">
         <v>86</v>
@@ -3201,14 +3216,14 @@
       <c r="G131" s="2"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
-  <sortState ref="C133:C138">
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C133:C138">
     <sortCondition ref="C133"/>
   </sortState>
   <conditionalFormatting sqref="B134">

</xml_diff>